<commit_message>
Append labels for binary tree
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konradfolwarski/PycharmProjects/Sztuczna_Inteligencja/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\AppData\Local\Programs\Python\Python39\Code\ESIProjekt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F6C25-8C98-F04A-88D3-847EA7008BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{E301AA55-92CB-D043-BB57-E2C331F4B07B}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16140"/>
   </bookViews>
   <sheets>
     <sheet name="WYNIK" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,9 +60,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>zarobki miesięczne</t>
-  </si>
-  <si>
     <t>&lt; 2000</t>
   </si>
   <si>
@@ -82,9 +78,6 @@
     <t>&lt; 2h temu</t>
   </si>
   <si>
-    <t>ilość osób spożywających pizze</t>
-  </si>
-  <si>
     <t>&gt; 2</t>
   </si>
   <si>
@@ -202,13 +195,19 @@
     <t>płeć</t>
   </si>
   <si>
-    <t>ostatni posiłek</t>
+    <t>zar. mies.</t>
+  </si>
+  <si>
+    <t>ost. posiłek</t>
+  </si>
+  <si>
+    <t>os. spoż. pizze</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,19 +937,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5F56FB-94BF-134E-86E7-FD6A0DF24147}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="102" width="4.33203125" customWidth="1"/>
+    <col min="3" max="102" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:102" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1471,7 @@
       <c r="CW2" s="6"/>
       <c r="CX2" s="6"/>
     </row>
-    <row r="3" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1606,7 +1605,7 @@
       <c r="CW3" s="6"/>
       <c r="CX3" s="6"/>
     </row>
-    <row r="4" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1740,7 +1739,7 @@
       <c r="CW4" s="6"/>
       <c r="CX4" s="6"/>
     </row>
-    <row r="5" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39"/>
       <c r="B5" s="10" t="s">
         <v>5</v>
@@ -1882,9 +1881,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -2086,7 +2085,7 @@
       <c r="CW6" s="6"/>
       <c r="CX6" s="6"/>
     </row>
-    <row r="7" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39"/>
       <c r="B7" s="10" t="s">
         <v>7</v>
@@ -2296,12 +2295,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:102" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:102" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -2462,10 +2461,10 @@
       <c r="CW8" s="6"/>
       <c r="CX8" s="6"/>
     </row>
-    <row r="9" spans="1:102" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:102" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38"/>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -2622,10 +2621,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39"/>
       <c r="B10" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -2816,12 +2815,12 @@
       <c r="CW10" s="18"/>
       <c r="CX10" s="18"/>
     </row>
-    <row r="11" spans="1:102" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:102" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="7"/>
@@ -3012,10 +3011,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:102" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:102" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38"/>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
@@ -3176,10 +3175,10 @@
       <c r="CW12" s="6"/>
       <c r="CX12" s="6"/>
     </row>
-    <row r="13" spans="1:102" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:102" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39"/>
       <c r="B13" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11">
@@ -3336,9 +3335,9 @@
       <c r="CW13" s="18"/>
       <c r="CX13" s="18"/>
     </row>
-    <row r="14" spans="1:102" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:102" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -3512,7 +3511,7 @@
       <c r="CW14" s="6"/>
       <c r="CX14" s="6"/>
     </row>
-    <row r="15" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="38"/>
       <c r="B15" s="2">
         <v>2</v>
@@ -3682,10 +3681,10 @@
       </c>
       <c r="CX15" s="6"/>
     </row>
-    <row r="16" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39"/>
       <c r="B16" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -3856,9 +3855,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:102" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:102" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="19"/>
@@ -3962,9 +3961,9 @@
       <c r="CW17" s="19"/>
       <c r="CX17" s="19"/>
     </row>
-    <row r="18" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="21">
@@ -4108,9 +4107,9 @@
       <c r="CW18" s="21"/>
       <c r="CX18" s="23"/>
     </row>
-    <row r="19" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="21"/>
@@ -4306,9 +4305,9 @@
       <c r="CW19" s="21"/>
       <c r="CX19" s="23"/>
     </row>
-    <row r="20" spans="1:102" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="24"/>
@@ -4480,29 +4479,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:102" x14ac:dyDescent="0.25">
       <c r="AA25" s="26"/>
       <c r="AB25" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:102" x14ac:dyDescent="0.25">
       <c r="W26" t="s">
+        <v>19</v>
+      </c>
+      <c r="X26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
         <v>21</v>
       </c>
-      <c r="X26" t="s">
+      <c r="AH27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="V27" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:102" x14ac:dyDescent="0.25">
       <c r="T28" s="26">
         <v>2</v>
       </c>
@@ -4510,78 +4509,78 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:102" x14ac:dyDescent="0.25">
       <c r="Q29" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH29" t="s">
         <v>25</v>
       </c>
-      <c r="R29" t="s">
+      <c r="AI29" t="s">
         <v>26</v>
       </c>
-      <c r="AH29" t="s">
+    </row>
+    <row r="31" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>21</v>
+      </c>
+      <c r="W31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:102" x14ac:dyDescent="0.25">
+      <c r="AX32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
         <v>27</v>
       </c>
-      <c r="AI29" t="s">
+      <c r="W33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="O31" t="s">
-        <v>23</v>
-      </c>
-      <c r="W31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="AX32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="L33" t="s">
-        <v>29</v>
-      </c>
-      <c r="W33" t="s">
-        <v>30</v>
-      </c>
       <c r="AK33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AZ33" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="34" spans="12:60" x14ac:dyDescent="0.25">
       <c r="AK34" s="26">
         <v>4</v>
       </c>
       <c r="AX34" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="AH35" t="s">
         <v>31</v>
       </c>
-      <c r="AY34" t="s">
+      <c r="AI35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="AH35" t="s">
+    <row r="36" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="AD36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW36" t="s">
         <v>33</v>
       </c>
-      <c r="AI35" t="s">
+      <c r="BH36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="AD36" t="s">
-        <v>23</v>
-      </c>
-      <c r="AW36" t="s">
-        <v>35</v>
-      </c>
-      <c r="BH36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="37" spans="12:60" x14ac:dyDescent="0.25">
       <c r="AA37" s="26">
         <v>6</v>
       </c>
@@ -4592,46 +4591,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="38" spans="12:60" x14ac:dyDescent="0.25">
       <c r="Y38" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU38" t="s">
         <v>37</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AV38" t="s">
         <v>38</v>
       </c>
-      <c r="AK38" t="s">
-        <v>24</v>
-      </c>
-      <c r="AU38" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV38" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="40" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="40" spans="12:60" x14ac:dyDescent="0.25">
       <c r="X40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AB40" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AL40" s="26">
         <v>7</v>
       </c>
       <c r="AU40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AY40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="41" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="41" spans="12:60" x14ac:dyDescent="0.25">
       <c r="AC41" s="26">
         <v>8</v>
       </c>
       <c r="AK41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AT41" s="26">
         <v>11</v>
@@ -4640,115 +4639,115 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="42" spans="12:60" x14ac:dyDescent="0.25">
       <c r="V42" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT42" t="s">
         <v>44</v>
       </c>
-      <c r="AA42" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB42" t="s">
+      <c r="AY42" t="s">
         <v>45</v>
       </c>
-      <c r="AT42" t="s">
+    </row>
+    <row r="43" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="AK43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="Z44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="Y45" t="s">
         <v>46</v>
       </c>
-      <c r="AY42" t="s">
+      <c r="AD45" t="s">
         <v>47</v>
       </c>
+      <c r="AI45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM45" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="43" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="AK43" t="s">
-        <v>23</v>
-      </c>
-      <c r="AN43" t="s">
-        <v>24</v>
+    <row r="46" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="AR46" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ46" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD46" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="44" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="Z44" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="Y45" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD45" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI45" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="AR46" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV46" t="s">
-        <v>24</v>
-      </c>
-      <c r="AZ46" t="s">
-        <v>35</v>
-      </c>
-      <c r="BD46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="12:60" x14ac:dyDescent="0.2">
+    <row r="47" spans="12:60" x14ac:dyDescent="0.25">
       <c r="AR47" s="26">
         <v>13</v>
       </c>
       <c r="AV47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="12:60" x14ac:dyDescent="0.25">
+      <c r="AP48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="12:60" x14ac:dyDescent="0.2">
-      <c r="AP48" t="s">
-        <v>50</v>
+    <row r="50" spans="40:48" x14ac:dyDescent="0.25">
+      <c r="AO50" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS50" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="50" spans="40:48" x14ac:dyDescent="0.2">
-      <c r="AO50" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="40:48" x14ac:dyDescent="0.2">
+    <row r="51" spans="40:48" x14ac:dyDescent="0.25">
       <c r="AN51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AU51" s="26">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="40:48" x14ac:dyDescent="0.2">
+    <row r="52" spans="40:48" x14ac:dyDescent="0.25">
       <c r="AS52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="54" spans="40:48" x14ac:dyDescent="0.2">
+    <row r="54" spans="40:48" x14ac:dyDescent="0.25">
       <c r="AR54" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AV54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="56" spans="40:48" x14ac:dyDescent="0.2">
+    <row r="56" spans="40:48" x14ac:dyDescent="0.25">
       <c r="AQ56" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AV56" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>